<commit_message>
Added bakery manufacturer filter test
</commit_message>
<xml_diff>
--- a/pn-testing-framework/input-data/Test_WashersPriceFilter.xlsx
+++ b/pn-testing-framework/input-data/Test_WashersPriceFilter.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="7">
   <si>
     <t>category</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Максимальная цена</t>
+  </si>
+  <si>
+    <t>filterLimit</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -102,9 +105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,9 +145,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +182,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,7 +217,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,22 +391,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -419,8 +422,11 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -434,10 +440,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -453,8 +462,11 @@
       <c r="E3" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -470,8 +482,11 @@
       <c r="E4" s="1">
         <v>4000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -487,8 +502,11 @@
       <c r="E5" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -504,8 +522,11 @@
       <c r="E6" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,8 +542,11 @@
       <c r="E7" s="1">
         <v>7000</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -538,8 +562,11 @@
       <c r="E8" s="1">
         <v>4000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -555,8 +582,11 @@
       <c r="E9" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -572,8 +602,11 @@
       <c r="E10" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -589,8 +622,11 @@
       <c r="E11" s="1">
         <v>7000</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -606,8 +642,11 @@
       <c r="E12" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -623,8 +662,11 @@
       <c r="E13" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -640,8 +682,11 @@
       <c r="E14" s="1">
         <v>7000</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -657,8 +702,11 @@
       <c r="E15" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -674,8 +722,11 @@
       <c r="E16" s="1">
         <v>7000</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -689,6 +740,9 @@
         <v>5</v>
       </c>
       <c r="E17" s="1">
+        <v>7000</v>
+      </c>
+      <c r="F17" s="1">
         <v>7000</v>
       </c>
     </row>

</xml_diff>